<commit_message>
update the testplaning document
</commit_message>
<xml_diff>
--- a/Testplanung_Kroll.xlsx
+++ b/Testplanung_Kroll.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheBestNew01\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\win10\Desktop\Mannschaftsverwaltung_ASP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B014DAE3-C98E-4398-A546-B99F60AA8FAD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5ED561E-BC20-458C-ADE3-1F9459019B7A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="1935" windowWidth="21600" windowHeight="11505"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Personenverwaltung" sheetId="1" r:id="rId1"/>
+    <sheet name="Mannschaftsverwaltung" sheetId="2" r:id="rId2"/>
+    <sheet name="Spiele" sheetId="3" r:id="rId3"/>
+    <sheet name="Tabellen" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,15 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t>Testplanung</t>
   </si>
   <si>
     <t>Durchführung</t>
-  </si>
-  <si>
-    <t>/Personen</t>
   </si>
   <si>
     <t>Link(Oberfläche)</t>
@@ -87,10 +87,6 @@
     <t>Darstellung der Mannschaften in einer Tabelle</t>
   </si>
   <si>
-    <t>Mannschaften sind in einer angemessenen Tabelle zu sehen.
-Durch Klicken eines Knopfes sollen die Personen sortierbar sein.</t>
-  </si>
-  <si>
     <t>/Spiele</t>
   </si>
   <si>
@@ -117,12 +113,31 @@
   </si>
   <si>
     <t>Durch Klicken des "Exportieren" Knopfes wird eine JSON-Datei heruntergeladen</t>
+  </si>
+  <si>
+    <t>Ergebnis</t>
+  </si>
+  <si>
+    <t>Hinzufügen von Mannschaften möglich</t>
+  </si>
+  <si>
+    <t>Durch Klicken auf den "Hinzufügen" Knopf öffnen sich Felder zur Eingabe einer neuen Mannschaft.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mannschaften sind in einer angemessenen Tabelle zu sehen.
+</t>
+  </si>
+  <si>
+    <t>Durch Klicken eines Knopfes sollen die Mannschaften sortierbar sein.</t>
+  </si>
+  <si>
+    <t>Sortieren der Mannschaft auf Knopfdruck</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -171,19 +186,19 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -498,11 +513,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:E33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C5:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,11 +526,12 @@
     <col min="3" max="3" width="34.42578125" customWidth="1"/>
     <col min="4" max="4" width="53.28515625" customWidth="1"/>
     <col min="5" max="5" width="74.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:5" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="5" spans="3:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>0</v>
@@ -523,247 +539,384 @@
       <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="7"/>
+      <c r="D8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="2"/>
-      <c r="D8" s="6" t="s">
+    <row r="9" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="7"/>
+      <c r="D9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E9" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="2"/>
-      <c r="D9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="2"/>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="7"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="7"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="7"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="7"/>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="7"/>
+      <c r="D14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="7"/>
+      <c r="D15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="7"/>
+      <c r="D16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="2"/>
-      <c r="D15" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="2"/>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="2"/>
-      <c r="D18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="2"/>
-      <c r="D20" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="2"/>
-      <c r="D21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="2"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="2"/>
-      <c r="D23" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="2"/>
-      <c r="D25" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C26" s="2"/>
-      <c r="D26" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="2"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="2"/>
-      <c r="D29" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C30" s="2"/>
-      <c r="D30" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="8"/>
-    </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="8"/>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="2"/>
-      <c r="D33" t="s">
-        <v>25</v>
-      </c>
-      <c r="E33" t="s">
-        <v>26</v>
-      </c>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="C28:C33"/>
+  <mergeCells count="5">
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="C7:C18"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="C7:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE3C3E3-974F-4D5C-B94B-11D25C5DD0BC}">
+  <dimension ref="C5:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="4" max="4" width="53.28515625" customWidth="1"/>
+    <col min="5" max="5" width="74.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="7"/>
+      <c r="D8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="7"/>
+      <c r="D9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="7"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="7"/>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C12" s="7"/>
+      <c r="D12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="7"/>
+      <c r="D13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C7:C13"/>
+    <mergeCell ref="E9:E10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC111A85-5543-46D2-BC52-9BA6D49A3729}">
+  <dimension ref="C5:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="4" max="4" width="53.28515625" customWidth="1"/>
+    <col min="5" max="5" width="74.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="7"/>
+      <c r="D8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="7"/>
+      <c r="D9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="7"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758C481B-E836-4438-ACAD-DCB9FAF0F891}">
+  <dimension ref="C5:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="4" max="4" width="53.28515625" customWidth="1"/>
+    <col min="5" max="5" width="74.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="7"/>
+      <c r="D8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="7"/>
+      <c r="D9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="7"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="7"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="7"/>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C7:C12"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
(after hours of trying to avoid this insane UI building approach) add teachers way of adding tablecontent and buttons to personenverwaltung
</commit_message>
<xml_diff>
--- a/Testplanung_Kroll.xlsx
+++ b/Testplanung_Kroll.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\win10\Desktop\Mannschaftsverwaltung_ASP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheBestNew01\Desktop\Mannschaftsverwaltung_ASP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5ED561E-BC20-458C-ADE3-1F9459019B7A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F4B069-DFD0-4603-ABB3-2879FEC8B66D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Personenverwaltung" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>Testplanung</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Sortieren der Mannschaft auf Knopfdruck</t>
+  </si>
+  <si>
+    <t>Bearbeiten/Löschen einer Person möglich</t>
+  </si>
+  <si>
+    <t>Durch Klicken der Knöpfe in der rechten Spalte wird eine Person bearbeitet/gelöscht</t>
   </si>
 </sst>
 </file>
@@ -192,13 +198,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -516,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C5:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,24 +574,24 @@
       <c r="D9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="8"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="8"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C12" s="7"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="8"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
@@ -619,17 +625,23 @@
       <c r="D16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" s="7"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
+      <c r="E17" s="8"/>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -700,14 +712,14 @@
       <c r="D9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
@@ -803,14 +815,14 @@
       <c r="D9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
@@ -836,7 +848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758C481B-E836-4438-ACAD-DCB9FAF0F891}">
   <dimension ref="C5:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9:D11"/>
     </sheetView>
   </sheetViews>
@@ -888,19 +900,19 @@
       <c r="D9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="8"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="8"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C12" s="7"/>

</xml_diff>